<commit_message>
exchange rates workflow created
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E345360-4652-44BD-A562-3ACA0F76EC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A632D6-155F-4F89-A397-59BF8E8325AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="10044" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -190,21 +190,12 @@
     <t>Royalties_BE001</t>
   </si>
   <si>
-    <t>BE001: N/A values found in 01 BobJ Loyd Analysis tab</t>
-  </si>
-  <si>
     <t>B4</t>
   </si>
   <si>
-    <t>BE002: Difference found between current and previous months' amount</t>
-  </si>
-  <si>
     <t>Royalties_BE002</t>
   </si>
   <si>
-    <t>BE003: Difference found between current and previous months' amount in Payment Schedule tab</t>
-  </si>
-  <si>
     <t>Royalties_BE003</t>
   </si>
   <si>
@@ -326,6 +317,48 @@
   </si>
   <si>
     <t>Royalties_YahooFinance_URL</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab</t>
+  </si>
+  <si>
+    <t>Exchange Rates</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab_CellRange1</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>I20</t>
+  </si>
+  <si>
+    <t>B22</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab_CellRange2</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab_CellRange3</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab_CellRange4</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab_CellRange5</t>
+  </si>
+  <si>
+    <t>C{0}</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRatesTab_Value1</t>
+  </si>
+  <si>
+    <t>P{0} - {1}</t>
   </si>
 </sst>
 </file>
@@ -754,7 +787,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -1783,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1970,7 +2003,7 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
@@ -1978,27 +2011,27 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -2006,7 +2039,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>45</v>
@@ -2014,10 +2047,10 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -2025,26 +2058,26 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2052,10 +2085,10 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
@@ -2064,26 +2097,26 @@
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1">
       <c r="A34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1">
       <c r="A35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
       <c r="A36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1">
@@ -2091,15 +2124,15 @@
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B39" s="2">
         <v>-2146826246</v>
@@ -2107,18 +2140,18 @@
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2127,7 +2160,7 @@
         <v>46</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
@@ -2135,7 +2168,7 @@
         <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
@@ -2144,76 +2177,113 @@
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1">
       <c r="A48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A50" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A53" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A55" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="50" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A52" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="55" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="60" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
+    </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
@@ -3159,6 +3229,16 @@
     <row r="1005" ht="14.25" customHeight="1"/>
     <row r="1006" ht="14.25" customHeight="1"/>
     <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
+    <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
+    <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
+    <row r="1016" ht="14.25" customHeight="1"/>
+    <row r="1017" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3170,8 +3250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3234,18 +3314,18 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
testing end to end
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A632D6-155F-4F89-A397-59BF8E8325AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB688A9-C9A4-41C0-9F75-C0CD518AB4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -280,24 +280,12 @@
     <t>BobJ - INT</t>
   </si>
   <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>A:F</t>
   </si>
   <si>
-    <t>Royalties_BobJINT_NAValue1</t>
-  </si>
-  <si>
-    <t>Royalties_BobJINT_NAValue2</t>
-  </si>
-  <si>
     <t>Lookups</t>
   </si>
   <si>
-    <t>B:B</t>
-  </si>
-  <si>
     <t>BE002: N/A values found in BobJ - INT tab</t>
   </si>
   <si>
@@ -359,6 +347,81 @@
   </si>
   <si>
     <t>P{0} - {1}</t>
+  </si>
+  <si>
+    <t>Royalties_RoyaltyMaster_TotalPremierFoodsTab</t>
+  </si>
+  <si>
+    <t>TOTAL PREMIER FOODS</t>
+  </si>
+  <si>
+    <t>Royalties_RoyaltyMaster_TotalPremierFoodsTab_CellRange</t>
+  </si>
+  <si>
+    <t>Check 2</t>
+  </si>
+  <si>
+    <t>Royalties_Check2Tab</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>D90:P90,D93:P97</t>
+  </si>
+  <si>
+    <t>Royalties_Check2Tab_CellRange</t>
+  </si>
+  <si>
+    <t>BE005: Amount difference found in Check 2</t>
+  </si>
+  <si>
+    <t>Royalties_BE004</t>
+  </si>
+  <si>
+    <t>Royalties_BE005</t>
+  </si>
+  <si>
+    <t>Royalties_UKINternationalRoyaltyStatementFileName</t>
+  </si>
+  <si>
+    <t>UK &amp; INTERNATIONAL ROYALTY STATEMENT - {0}</t>
+  </si>
+  <si>
+    <t>Brand HL4 - Reclass,Check 1,Check 2,Lookups</t>
+  </si>
+  <si>
+    <t>Royalties_UKINternationalRoyaltyStatement_ExcludedWorksheets</t>
+  </si>
+  <si>
+    <t>Royalties_CadburyFolderPath</t>
+  </si>
+  <si>
+    <t>BE007: Amount difference exceeds +/-200k</t>
+  </si>
+  <si>
+    <t>Royalties_BE006</t>
+  </si>
+  <si>
+    <t>Royalties_BE007</t>
+  </si>
+  <si>
+    <t>BE006: Variance in calculated Royalty Totals</t>
+  </si>
+  <si>
+    <t>BE004: Exchange rate could not be extracted</t>
+  </si>
+  <si>
+    <t>Royalties_BobJInt_NAValue1</t>
+  </si>
+  <si>
+    <t>Royalties_BobJInt_NAValue2</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>B2</t>
   </si>
 </sst>
 </file>
@@ -376,6 +439,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -1816,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1017"/>
+  <dimension ref="A1:Z1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2069,7 +2133,7 @@
         <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
@@ -2108,7 +2172,7 @@
         <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>80</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
@@ -2116,7 +2180,7 @@
         <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1">
@@ -2124,7 +2188,7 @@
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>67</v>
@@ -2132,7 +2196,7 @@
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="B39" s="2">
         <v>-2146826246</v>
@@ -2160,7 +2224,7 @@
         <v>46</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
@@ -2168,7 +2232,7 @@
         <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
@@ -2177,18 +2241,18 @@
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
@@ -2197,50 +2261,50 @@
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
@@ -2249,59 +2313,138 @@
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A62" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A65" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A66" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A68" t="s">
         <v>49</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B68" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A61" t="s">
+    <row r="69" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
         <v>51</v>
       </c>
-      <c r="B61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A62" t="s">
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A70" t="s">
         <v>52</v>
       </c>
-      <c r="B62" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+      <c r="B70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A73" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A74" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -3239,6 +3382,14 @@
     <row r="1015" ht="14.25" customHeight="1"/>
     <row r="1016" ht="14.25" customHeight="1"/>
     <row r="1017" ht="14.25" customHeight="1"/>
+    <row r="1018" ht="14.25" customHeight="1"/>
+    <row r="1019" ht="14.25" customHeight="1"/>
+    <row r="1020" ht="14.25" customHeight="1"/>
+    <row r="1021" ht="14.25" customHeight="1"/>
+    <row r="1022" ht="14.25" customHeight="1"/>
+    <row r="1023" ht="14.25" customHeight="1"/>
+    <row r="1024" ht="14.25" customHeight="1"/>
+    <row r="1025" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3251,7 +3402,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3322,13 +3473,20 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add send email workflow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB688A9-C9A4-41C0-9F75-C0CD518AB4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13075EF2-4061-475C-A0B4-798426EB1911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="183">
   <si>
     <t>Name</t>
   </si>
@@ -422,6 +422,194 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_TenantID</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_Account</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_CadburySubject</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_Inbox</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_To</t>
+  </si>
+  <si>
+    <t>Royalties_BE001_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Subject for BE001</t>
+  </si>
+  <si>
+    <t>Royalties_BE001_Mail_Body</t>
+  </si>
+  <si>
+    <t>Body for BE001</t>
+  </si>
+  <si>
+    <t>Royalties_BE002_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Subject for BE002</t>
+  </si>
+  <si>
+    <t>Royalties_BE002_Mail_Body</t>
+  </si>
+  <si>
+    <t>Body for BE002</t>
+  </si>
+  <si>
+    <t>Royalties_BE003_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_BE003_Mail_Body</t>
+  </si>
+  <si>
+    <t>Royalties_BE004_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_BE004_Mail_Body</t>
+  </si>
+  <si>
+    <t>Royalties_BE005_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_BE005_Mail_Body</t>
+  </si>
+  <si>
+    <t>Royalties_BE006_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_BE006_Mail_Body</t>
+  </si>
+  <si>
+    <t>Royalties_BE007_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_BE007_Mail_Body</t>
+  </si>
+  <si>
+    <t>Subject for BE003</t>
+  </si>
+  <si>
+    <t>Body for BE003</t>
+  </si>
+  <si>
+    <t>Subject for BE004</t>
+  </si>
+  <si>
+    <t>Body for BE006</t>
+  </si>
+  <si>
+    <t>Body for BE007</t>
+  </si>
+  <si>
+    <t>Body for BE004</t>
+  </si>
+  <si>
+    <t>Subject for BE005</t>
+  </si>
+  <si>
+    <t>Body for BE005</t>
+  </si>
+  <si>
+    <t>Subject for BE006</t>
+  </si>
+  <si>
+    <t>Subject for BE007</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - Amount difference found in Check 1</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - Exchange rate could not be extracted</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - Amount difference found in Check 2</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - Variance in calculated Royalty Totals</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - Amount difference exceeds +/-200k</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - N/A values found in BobJ - UK tab</t>
+  </si>
+  <si>
+    <t>Royalties_Success_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Royalties_Success_Mail_Body</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury - Royalty Master {0}</t>
+  </si>
+  <si>
+    <t>Subject for Successful run</t>
+  </si>
+  <si>
+    <t>Body for Successful run</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_AppIDAndSecret</t>
+  </si>
+  <si>
+    <t>UiPath_O365_Mail_Send_and_Receive</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found N/A values in BobJ - UK tab. It added the values to the Royalty Master Template, Brand HL4 - Reclass tab.&lt;/p&gt;
+  &lt;p&gt;Please add the necessary information to the Template and restart the process.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt; 
+ &lt;p&gt;The robot found N/A values in BobJ - INT tab. It added the values to the Royalty Master Template, Brand HL4 - Reclass and Lookups tabs.&lt;/p&gt;
+  &lt;p&gt;Please add the necessary information to the Template and restart the process.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found differences in the values found in Check 1 tab.&lt;/p&gt;
+  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot was unable to extract the exchange rate from the Yahoo Finance website.&lt;/p&gt;
+  &lt;p&gt;Please add the necessary information to the Exchange Rates tab.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found differences in the values found in Check 2 tab.&lt;/p&gt;
+  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found differences in the variance calculated in the LL Working file.&lt;/p&gt;
+  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found differences between the current fiscal period and the previous one that exceeds +/-200k.&lt;/p&gt;
+  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot created the Royalty Master file and the UK and International Royalty Statement file and attached them to this email.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -801,7 +989,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -879,7 +1067,14 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1880,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1025"/>
+  <dimension ref="A1:Z1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2363,7 +2558,7 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+    <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>114</v>
       </c>
@@ -2371,7 +2566,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+    <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>117</v>
       </c>
@@ -2379,11 +2574,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+    <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:2" ht="14.25" customHeight="1">
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -2391,7 +2586,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.25" customHeight="1">
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -2399,7 +2594,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.25" customHeight="1">
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" t="s">
         <v>52</v>
       </c>
@@ -2407,7 +2602,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2415,7 +2610,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" t="s">
         <v>113</v>
       </c>
@@ -2423,7 +2618,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.25" customHeight="1">
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" t="s">
         <v>120</v>
       </c>
@@ -2431,7 +2626,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.25" customHeight="1">
+    <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>121</v>
       </c>
@@ -2439,28 +2634,188 @@
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A76" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A77" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A78" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A79" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A80" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A81" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A82" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A83" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A84" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A85" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C85" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A86" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A87" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A88" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A89" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="91" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A92" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="94" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="95" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="96" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="97" ht="14.25" customHeight="1"/>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>
@@ -3389,7 +3744,6 @@
     <row r="1022" ht="14.25" customHeight="1"/>
     <row r="1023" ht="14.25" customHeight="1"/>
     <row r="1024" ht="14.25" customHeight="1"/>
-    <row r="1025" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3399,10 +3753,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3453,44 +3807,68 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"Integer.Parse(in_Config("&amp;""""&amp;A2&amp;""""&amp;").ToString)"</f>
-        <v>Integer.Parse(in_Config("Tenant ID").ToString)</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>118</v>
+      <c r="A5" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4481,7 +4859,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LL workings development + testing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13075EF2-4061-475C-A0B4-798426EB1911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F06A91-6181-40FF-8990-3096387C110A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="204">
   <si>
     <t>Name</t>
   </si>
@@ -380,15 +380,6 @@
   </si>
   <si>
     <t>Royalties_BE005</t>
-  </si>
-  <si>
-    <t>Royalties_UKINternationalRoyaltyStatementFileName</t>
-  </si>
-  <si>
-    <t>UK &amp; INTERNATIONAL ROYALTY STATEMENT - {0}</t>
-  </si>
-  <si>
-    <t>Brand HL4 - Reclass,Check 1,Check 2,Lookups</t>
   </si>
   <si>
     <t>Royalties_UKINternationalRoyaltyStatement_ExcludedWorksheets</t>
@@ -610,6 +601,78 @@
     <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
   &lt;p&gt;The robot created the Royalty Master file and the UK and International Royalty Statement file and attached them to this email.&lt;/p&gt;
   &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Royalties_UKInternationalRoyaltyStatementFileName</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_InboxCadbury</t>
+  </si>
+  <si>
+    <t>Data\vbaCodes.txt</t>
+  </si>
+  <si>
+    <t>DeleteSheet</t>
+  </si>
+  <si>
+    <t>Royalties_VBACodes</t>
+  </si>
+  <si>
+    <t>Royalties_VBAFunction_DeleteSheet</t>
+  </si>
+  <si>
+    <t>Check 1,Check 2</t>
+  </si>
+  <si>
+    <t>Royalties_ExchangeRates_CaptureFileName</t>
+  </si>
+  <si>
+    <t>InsertPicture</t>
+  </si>
+  <si>
+    <t>Royalties_VBAFunction_InsertPicture</t>
+  </si>
+  <si>
+    <t>exchangeRate.jpg</t>
+  </si>
+  <si>
+    <t>Royalties_BobJLL_CheckTab</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Royalties_BobJLL_CheckTab_CellRange</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Royalties_LLWorkings_CellRange</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>J82</t>
+  </si>
+  <si>
+    <t>Royalties_LLWorkings_CellRangeTNV</t>
+  </si>
+  <si>
+    <t>K82</t>
+  </si>
+  <si>
+    <t>Royalties_LLWorkings_CellRangeRoyalty</t>
+  </si>
+  <si>
+    <t>Royalties_LLWorkings_Check</t>
+  </si>
+  <si>
+    <t>K84</t>
+  </si>
+  <si>
+    <t>Royalties_LLWorkings_CellRangeRoyaltyVariance</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1052,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1069,10 +1132,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2075,10 +2138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1024"/>
+  <dimension ref="A1:Z1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2367,7 +2430,7 @@
         <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
@@ -2383,7 +2446,7 @@
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>67</v>
@@ -2391,7 +2454,7 @@
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B39" s="2">
         <v>-2146826246</v>
@@ -2427,7 +2490,7 @@
         <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
@@ -2539,299 +2602,378 @@
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A62" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1">
       <c r="A63" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A64" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A66" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A67" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A69" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A70" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A71" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A72" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A73" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A75" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A66" s="2" t="s">
+      <c r="B75" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A78" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A80" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A82" t="s">
         <v>117</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A68" t="s">
-        <v>49</v>
-      </c>
-      <c r="B68" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B69" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A70" t="s">
-        <v>52</v>
-      </c>
-      <c r="B70" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A71" t="s">
-        <v>112</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A72" t="s">
-        <v>113</v>
-      </c>
-      <c r="B72" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A73" t="s">
-        <v>120</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A74" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B74" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="76" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A76" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C76" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A77" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C77" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A78" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A79" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C79" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A80" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C80" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A81" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C81" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A82" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C82" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C83" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A84" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C84" t="s">
-        <v>158</v>
-      </c>
-    </row>
+        <v>118</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="85" spans="1:3" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>179</v>
+        <v>131</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C85" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>165</v>
+        <v>133</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>172</v>
       </c>
       <c r="C86" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>180</v>
+        <v>135</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C87" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>166</v>
+        <v>137</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="C88" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C89" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A90" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A91" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C91" t="s">
         <v>151</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" t="s">
+    </row>
+    <row r="92" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A92" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C92" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A93" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C93" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A94" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C94" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="91" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A91" t="s">
+    <row r="95" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A95" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C95" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A96" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A97" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C97" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A98" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="100" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A100" t="s">
+        <v>165</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C100" t="s">
         <v>168</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C91" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A92" t="s">
+    </row>
+    <row r="101" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A101" t="s">
+        <v>166</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C101" t="s">
         <v>169</v>
       </c>
-      <c r="B92" s="3" t="s">
+    </row>
+    <row r="102" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="103" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A103" t="s">
+        <v>184</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C92" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="94" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="95" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="96" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="104" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A104" t="s">
+        <v>185</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A105" t="s">
+        <v>189</v>
+      </c>
+      <c r="B105" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A106" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="108" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="109" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="110" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="113" ht="14.25" customHeight="1"/>
     <row r="114" ht="14.25" customHeight="1"/>
     <row r="115" ht="14.25" customHeight="1"/>
@@ -3744,6 +3886,15 @@
     <row r="1022" ht="14.25" customHeight="1"/>
     <row r="1023" ht="14.25" customHeight="1"/>
     <row r="1024" ht="14.25" customHeight="1"/>
+    <row r="1025" ht="14.25" customHeight="1"/>
+    <row r="1026" ht="14.25" customHeight="1"/>
+    <row r="1027" ht="14.25" customHeight="1"/>
+    <row r="1028" ht="14.25" customHeight="1"/>
+    <row r="1029" ht="14.25" customHeight="1"/>
+    <row r="1030" ht="14.25" customHeight="1"/>
+    <row r="1031" ht="14.25" customHeight="1"/>
+    <row r="1032" ht="14.25" customHeight="1"/>
+    <row r="1033" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3756,7 +3907,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3823,53 +3974,60 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
+        <v>180</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>131</v>
+      <c r="A7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
latest changes after uat review
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F9F998-2245-4962-AF1B-E2EC22727450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EA8CB5-27B5-46F3-9F4C-1758BDD32B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -603,31 +603,19 @@
     <t>Royalties_BobJLL_CheckTab_CellRange</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
     <t>Royalties_LLWorkings_CellRange</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>J82</t>
   </si>
   <si>
     <t>Royalties_LLWorkings_CellRangeTNV</t>
   </si>
   <si>
-    <t>K82</t>
-  </si>
-  <si>
     <t>Royalties_LLWorkings_CellRangeRoyalty</t>
   </si>
   <si>
     <t>Royalties_LLWorkings_Check</t>
-  </si>
-  <si>
-    <t>K84</t>
   </si>
   <si>
     <t>Royalties_LLWorkings_CellRangeRoyaltyVariance</t>
@@ -697,25 +685,67 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
-  &lt;p&gt;The robot found differences between the current fiscal period and the previous one that exceeds +/-200k in file Royalty Master {0}.&lt;/p&gt;
-  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
-  &lt;p&gt;Thank you!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
   &lt;p&gt;The robot found missing values in the I&amp;I Actuals {0}.&lt;/p&gt;
   &lt;p&gt;Please add the missing values in the Lookups tab, in the I&amp;I Actuals Template file and restart the process .&lt;/p&gt;
   &lt;p&gt;Thank you!&lt;/p&gt;</t>
   </si>
   <si>
     <t>Royalty Cadbury - N/A values found in BobJ - INT tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found differences between the current fiscal period and the previous one that exceeds +/-200k in file Royalty Master {0}.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>I82</t>
+  </si>
+  <si>
+    <t>J84</t>
+  </si>
+  <si>
+    <t>Royalties_SE_Mail_Subject</t>
+  </si>
+  <si>
+    <t>Subject for SE</t>
+  </si>
+  <si>
+    <t>Body for SE</t>
+  </si>
+  <si>
+    <t>Royalty Cadbury Performer - System Exception</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;An error has occurred while trying to run the Performer:&lt;/p&gt;
+&lt;p&gt;{0}&lt;/p&gt;
+  &lt;p&gt;Please check the logs to find the root cause and also notify the SMEs if the error is impacting any deadline.&lt;/p&gt;
+ &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Royalties_Mail_SE_To</t>
+  </si>
+  <si>
+    <t>ActivateFirstWorksheet</t>
+  </si>
+  <si>
+    <t>Royalties_VBAFunction_ActivateFirstWorksheet</t>
+  </si>
+  <si>
+    <t>Royalties_SE_Mail_Body</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,000"/>
+  </numFmts>
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -740,16 +770,201 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF00CC00"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF33CC33"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF9900"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1F5FB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EFF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6F9C1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABEDA5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94D88F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFDBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFB8C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF843"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF988C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6758"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7CFE8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3D6EB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -757,9 +972,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyBorder="0">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyBorder="0">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="3" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="2" applyNumberFormat="0" applyBorder="0">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="3" applyNumberFormat="0" applyBorder="0">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -772,8 +1188,45 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="38">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="SAPBorder" xfId="19" xr:uid="{BD44032D-0D1A-4307-B195-B918B4B16D63}"/>
+    <cellStyle name="SAPDataCell" xfId="2" xr:uid="{0439CA0C-AB38-4AB7-8164-18D720D849C9}"/>
+    <cellStyle name="SAPDataTotalCell" xfId="3" xr:uid="{1F54364F-3D34-4E3A-AB3B-0F54C407DBC2}"/>
+    <cellStyle name="SAPDimensionCell" xfId="1" xr:uid="{3792B803-5AE5-43A3-A2B8-95EB42FF12CA}"/>
+    <cellStyle name="SAPEditableDataCell" xfId="4" xr:uid="{D36835E5-7038-4553-9B54-37B05C3A75F7}"/>
+    <cellStyle name="SAPEditableDataTotalCell" xfId="7" xr:uid="{02DB303C-0D58-41E6-95B8-37EE03BB5570}"/>
+    <cellStyle name="SAPEmphasized" xfId="27" xr:uid="{87EF4E66-B659-4614-9266-C265F42C5CAA}"/>
+    <cellStyle name="SAPEmphasizedEditableDataCell" xfId="29" xr:uid="{067D781C-3A49-4F3C-A91B-9B96A846C051}"/>
+    <cellStyle name="SAPEmphasizedEditableDataTotalCell" xfId="30" xr:uid="{D020270B-519D-4034-AE24-CD2F749405C6}"/>
+    <cellStyle name="SAPEmphasizedLockedDataCell" xfId="33" xr:uid="{5673E949-486A-4C6F-A586-B06B6E77183F}"/>
+    <cellStyle name="SAPEmphasizedLockedDataTotalCell" xfId="34" xr:uid="{08DEA685-97CD-4E49-AAE3-4598301A684C}"/>
+    <cellStyle name="SAPEmphasizedReadonlyDataCell" xfId="31" xr:uid="{60F43C70-F687-4495-AAA4-45577EC91565}"/>
+    <cellStyle name="SAPEmphasizedReadonlyDataTotalCell" xfId="32" xr:uid="{48968376-ED52-49C8-8F1E-DE3D612D4C02}"/>
+    <cellStyle name="SAPEmphasizedTotal" xfId="28" xr:uid="{3F58B8CC-6E2A-4331-9CF5-7FF37F3261EC}"/>
+    <cellStyle name="SAPError" xfId="37" xr:uid="{C8596C44-D83C-4252-AA4F-830128471DB6}"/>
+    <cellStyle name="SAPExceptionLevel1" xfId="10" xr:uid="{715CE561-F9B7-4D27-ACAB-FEA0E5ED061E}"/>
+    <cellStyle name="SAPExceptionLevel2" xfId="11" xr:uid="{FE31ECC5-0CC7-44DE-80D0-DFAF5B8B95C7}"/>
+    <cellStyle name="SAPExceptionLevel3" xfId="12" xr:uid="{E1E71FDF-EF35-4165-9897-3DB1069BEC5B}"/>
+    <cellStyle name="SAPExceptionLevel4" xfId="13" xr:uid="{5C984276-65C8-42A7-88DF-D5D668B381FA}"/>
+    <cellStyle name="SAPExceptionLevel5" xfId="14" xr:uid="{DE370214-9ABF-4E65-A0CB-7676F453C1CE}"/>
+    <cellStyle name="SAPExceptionLevel6" xfId="15" xr:uid="{1E422384-680E-4CAE-99C0-DBB47E2A5C5F}"/>
+    <cellStyle name="SAPExceptionLevel7" xfId="16" xr:uid="{02FB1D76-EFAD-444F-8261-F358281D7FDC}"/>
+    <cellStyle name="SAPExceptionLevel8" xfId="17" xr:uid="{361303A2-F79B-4662-81CE-15C85C70CBCA}"/>
+    <cellStyle name="SAPExceptionLevel9" xfId="18" xr:uid="{244A4D25-471E-4395-8D9C-9757E7052CB1}"/>
+    <cellStyle name="SAPFormula" xfId="36" xr:uid="{082D383A-F21A-46DF-A4C8-18FD4538C95D}"/>
+    <cellStyle name="SAPHierarchyCell0" xfId="22" xr:uid="{11FC9BD9-C120-4C7E-A7C7-E7140BDA7562}"/>
+    <cellStyle name="SAPHierarchyCell1" xfId="23" xr:uid="{BCD35E0C-EC1A-4874-977B-2CD00F18E0DF}"/>
+    <cellStyle name="SAPHierarchyCell2" xfId="24" xr:uid="{990D1453-ACB5-4572-935A-D35BFA154D28}"/>
+    <cellStyle name="SAPHierarchyCell3" xfId="25" xr:uid="{4C758056-47AF-402A-9DEA-FEE642964EC3}"/>
+    <cellStyle name="SAPHierarchyCell4" xfId="26" xr:uid="{7830B144-458C-4045-B803-B396D9C6DCED}"/>
+    <cellStyle name="SAPLockedDataCell" xfId="6" xr:uid="{167D0EF5-F181-4A28-8FE3-41497EB1EE5E}"/>
+    <cellStyle name="SAPLockedDataTotalCell" xfId="9" xr:uid="{EA7D72AC-B2A6-47FB-903D-F11507FB264D}"/>
+    <cellStyle name="SAPMemberCell" xfId="20" xr:uid="{D6645FC4-C0E3-4B7A-994A-2C141F21D4FE}"/>
+    <cellStyle name="SAPMemberTotalCell" xfId="21" xr:uid="{6C343C7A-A30E-4309-8797-B7554FB811DD}"/>
+    <cellStyle name="SAPMessageText" xfId="35" xr:uid="{BC973795-AAF7-4092-B2A7-8662E8885C88}"/>
+    <cellStyle name="SAPReadonlyDataCell" xfId="5" xr:uid="{6E464540-86EE-4EBE-AF36-1E525C4C885A}"/>
+    <cellStyle name="SAPReadonlyDataTotalCell" xfId="8" xr:uid="{F73A8336-7BE4-47A1-9DDE-649B2956CF9F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2169,15 +2622,18 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1036"/>
+  <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2394,10 +2850,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -2674,7 +3130,7 @@
         <v>184</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.25" customHeight="1">
@@ -2682,7 +3138,7 @@
         <v>186</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.25" customHeight="1">
@@ -2691,7 +3147,7 @@
     </row>
     <row r="70" spans="1:2" ht="14.25" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>185</v>
@@ -2699,34 +3155,34 @@
     </row>
     <row r="71" spans="1:2" ht="14.25" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.25" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.25" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1">
@@ -2803,10 +3259,10 @@
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2826,7 +3282,7 @@
         <v>133</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C88" t="s">
         <v>134</v>
@@ -2837,7 +3293,7 @@
         <v>135</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C89" t="s">
         <v>136</v>
@@ -2848,7 +3304,7 @@
         <v>137</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C90" t="s">
         <v>138</v>
@@ -2870,7 +3326,7 @@
         <v>140</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C92" t="s">
         <v>150</v>
@@ -2892,7 +3348,7 @@
         <v>142</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C94" t="s">
         <v>154</v>
@@ -2914,7 +3370,7 @@
         <v>144</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C96" t="s">
         <v>156</v>
@@ -2936,7 +3392,7 @@
         <v>146</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C98" t="s">
         <v>152</v>
@@ -2944,24 +3400,24 @@
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C99" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C100" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1">
@@ -2980,7 +3436,7 @@
         <v>148</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C102" t="s">
         <v>153</v>
@@ -3035,31 +3491,58 @@
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
+        <v>221</v>
+      </c>
+      <c r="B109" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A110" t="s">
         <v>180</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="112" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="112" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A112" t="s">
+        <v>214</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C112" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A113" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C113" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="115" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="116" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="117" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="118" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="119" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="120" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="121" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="122" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="123" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="124" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="125" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="126" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="127" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="128" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="129" ht="14.25" customHeight="1"/>
     <row r="130" ht="14.25" customHeight="1"/>
     <row r="131" ht="14.25" customHeight="1"/>
@@ -3968,10 +4451,14 @@
     <row r="1034" ht="14.25" customHeight="1"/>
     <row r="1035" ht="14.25" customHeight="1"/>
     <row r="1036" ht="14.25" customHeight="1"/>
+    <row r="1037" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -3980,7 +4467,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4101,7 +4588,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -5093,5 +5587,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
period run is calendaristic month
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EA8CB5-27B5-46F3-9F4C-1758BDD32B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7888F7A0-D004-45A2-92B9-BD39894231BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,12 +679,6 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
-  &lt;p&gt;The robot found differences in the variance calculated in the LL Workings {0}.&lt;/p&gt;
-  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
-  &lt;p&gt;Thank you!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
   &lt;p&gt;The robot found missing values in the I&amp;I Actuals {0}.&lt;/p&gt;
   &lt;p&gt;Please add the missing values in the Lookups tab, in the I&amp;I Actuals Template file and restart the process .&lt;/p&gt;
   &lt;p&gt;Thank you!&lt;/p&gt;</t>
@@ -736,6 +730,12 @@
   </si>
   <si>
     <t>Royalties_SE_Mail_Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
+  &lt;p&gt;The robot found differences in the variance calculated in the Cadbury Royalty check report BOBJ {0}.&lt;/p&gt;
+  &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
+  &lt;p&gt;Thank you!&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -2632,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3158,7 +3158,7 @@
         <v>187</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.25" customHeight="1">
@@ -3166,7 +3166,7 @@
         <v>189</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1">
@@ -3182,7 +3182,7 @@
         <v>192</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1">
@@ -3293,7 +3293,7 @@
         <v>135</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C89" t="s">
         <v>136</v>
@@ -3392,7 +3392,7 @@
         <v>146</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C98" t="s">
         <v>152</v>
@@ -3414,7 +3414,7 @@
         <v>198</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C100" t="s">
         <v>201</v>
@@ -3436,7 +3436,7 @@
         <v>148</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C102" t="s">
         <v>153</v>
@@ -3491,10 +3491,10 @@
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B109" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1">
@@ -3508,24 +3508,24 @@
     <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="112" spans="1:3" ht="14.25" customHeight="1">
       <c r="A112" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C112" t="s">
         <v>214</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C112" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1">
       <c r="A113" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C113" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4590,10 +4590,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
changes after testing with sandip
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7888F7A0-D004-45A2-92B9-BD39894231BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D25CCD3-94EF-4A0B-9A41-D44593D83ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="221">
   <si>
     <t>Name</t>
   </si>
@@ -597,16 +597,10 @@
     <t>Royalties_BobJLL_CheckTab</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>Royalties_BobJLL_CheckTab_CellRange</t>
   </si>
   <si>
     <t>Royalties_LLWorkings_CellRange</t>
-  </si>
-  <si>
-    <t>J82</t>
   </si>
   <si>
     <t>Royalties_LLWorkings_CellRangeTNV</t>
@@ -690,15 +684,6 @@
     <t xml:space="preserve"> &lt;p&gt;Hi,&lt;/p&gt;
   &lt;p&gt;The robot found differences between the current fiscal period and the previous one that exceeds +/-200k in file Royalty Master {0}.&lt;/p&gt;
   &lt;p&gt;Thank you!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>I82</t>
-  </si>
-  <si>
-    <t>J84</t>
   </si>
   <si>
     <t>Royalties_SE_Mail_Subject</t>
@@ -736,6 +721,15 @@
   &lt;p&gt;The robot found differences in the variance calculated in the Cadbury Royalty check report BOBJ {0}.&lt;/p&gt;
   &lt;p&gt;Make sure that you check where the differences come from.&lt;/p&gt;
   &lt;p&gt;Thank you!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>I63</t>
+  </si>
+  <si>
+    <t>J63</t>
+  </si>
+  <si>
+    <t>J65</t>
   </si>
 </sst>
 </file>
@@ -2632,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2850,10 +2844,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -3135,10 +3129,10 @@
     </row>
     <row r="68" spans="1:2" ht="14.25" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.25" customHeight="1">
@@ -3147,42 +3141,42 @@
     </row>
     <row r="70" spans="1:2" ht="14.25" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.25" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.25" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.25" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1">
@@ -3259,10 +3253,10 @@
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3282,7 +3276,7 @@
         <v>133</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C88" t="s">
         <v>134</v>
@@ -3293,7 +3287,7 @@
         <v>135</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C89" t="s">
         <v>136</v>
@@ -3304,7 +3298,7 @@
         <v>137</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C90" t="s">
         <v>138</v>
@@ -3326,7 +3320,7 @@
         <v>140</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C92" t="s">
         <v>150</v>
@@ -3348,7 +3342,7 @@
         <v>142</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C94" t="s">
         <v>154</v>
@@ -3370,7 +3364,7 @@
         <v>144</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C96" t="s">
         <v>156</v>
@@ -3392,7 +3386,7 @@
         <v>146</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C98" t="s">
         <v>152</v>
@@ -3400,24 +3394,24 @@
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="C99" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1">
@@ -3436,7 +3430,7 @@
         <v>148</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C102" t="s">
         <v>153</v>
@@ -3491,10 +3485,10 @@
     </row>
     <row r="109" spans="1:3" ht="14.25" customHeight="1">
       <c r="A109" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1">
@@ -3508,24 +3502,24 @@
     <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="112" spans="1:3" ht="14.25" customHeight="1">
       <c r="A112" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C112" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.25" customHeight="1">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C113" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.25" customHeight="1"/>
@@ -4590,10 +4584,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
fixed errors from LL workings and bobj int
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Royalties_CadburyPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D25CCD3-94EF-4A0B-9A41-D44593D83ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE8BD5F-41C0-42DB-A95F-202780987B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -730,6 +730,12 @@
   </si>
   <si>
     <t>J65</t>
+  </si>
+  <si>
+    <t>ExtendFormula</t>
+  </si>
+  <si>
+    <t>Royalties_VBAFunction_ExtendFormula</t>
   </si>
 </sst>
 </file>
@@ -2626,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3499,7 +3505,14 @@
         <v>183</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="111" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A111" t="s">
+        <v>222</v>
+      </c>
+      <c r="B111" t="s">
+        <v>221</v>
+      </c>
+    </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1">
       <c r="A112" t="s">
         <v>208</v>

</xml_diff>